<commit_message>
removed distinction between argument and statement
</commit_message>
<xml_diff>
--- a/MirrorMe/Arguments.xlsx
+++ b/MirrorMe/Arguments.xlsx
@@ -10,14 +10,13 @@
     <sheet name="Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Claims" sheetId="3" r:id="rId2"/>
     <sheet name="Statements" sheetId="5" r:id="rId3"/>
-    <sheet name="Arguments" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>7148691</t>
   </si>
@@ -28,9 +27,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Argument</t>
-  </si>
-  <si>
     <t>Case</t>
   </si>
   <si>
@@ -55,9 +51,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>[Argument]</t>
-  </si>
-  <si>
     <t>[Case]</t>
   </si>
   <si>
@@ -143,12 +136,6 @@
   </si>
   <si>
     <t>s8</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
   </si>
   <si>
     <t>Art 7:610 lid 1 BW</t>
@@ -525,57 +512,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -595,44 +582,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -642,232 +629,170 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
+      <c r="F10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The user can now build an argumentation interactively.
</commit_message>
<xml_diff>
--- a/MirrorMe/Arguments.xlsx
+++ b/MirrorMe/Arguments.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Claims" sheetId="3" r:id="rId2"/>
     <sheet name="Statements" sheetId="5" r:id="rId3"/>
+    <sheet name="Arguments" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
   <si>
     <t>7148691</t>
   </si>
@@ -42,9 +43,6 @@
     <t>LegalGround</t>
   </si>
   <si>
-    <t>Moment</t>
-  </si>
-  <si>
     <t>Statement</t>
   </si>
   <si>
@@ -75,9 +73,6 @@
     <t>madeBy</t>
   </si>
   <si>
-    <t>moment</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
@@ -117,9 +112,6 @@
     <t>ontslag</t>
   </si>
   <si>
-    <t>Het ontslag is onterecht</t>
-  </si>
-  <si>
     <t>LegalThing</t>
   </si>
   <si>
@@ -138,32 +130,144 @@
     <t>s8</t>
   </si>
   <si>
-    <t>Art 7:610 lid 1 BW</t>
-  </si>
-  <si>
-    <t>Eiser had recht op voldoening van loon ten bedrage van €1235,- op 22 oktober 2015</t>
-  </si>
-  <si>
-    <t>Gedaagde heeft het loon niet voldaan op 27 oktober 2015</t>
-  </si>
-  <si>
-    <t>27 oktober 2015 is de derde werkdag na 22 oktober 2015</t>
-  </si>
-  <si>
-    <t>Er is sprake van vertraging, omdat het loon niet voldaan is op de derde werkdag na die waarop de voldoening had moeten geschieden.</t>
-  </si>
-  <si>
-    <t>Deze vertraging is toe te rekenen aan de gedaagde.</t>
-  </si>
-  <si>
     <t>Art 7:625 lid 1 BW</t>
+  </si>
+  <si>
+    <t>Dit niet-voldoen is toe te rekenen aan de werkgever.</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>27 oktober 2015 is de derde werkdag na 22 oktober 2015.</t>
+  </si>
+  <si>
+    <t>Art 7:623 BW</t>
+  </si>
+  <si>
+    <t>Art 7:624 lid 1 BW</t>
+  </si>
+  <si>
+    <t>De voldoening van dit loon had moeten geschieden op 22 oktober 2015.</t>
+  </si>
+  <si>
+    <t>Dit loon is niet voldaan op 27 oktober 2015.</t>
+  </si>
+  <si>
+    <t>datumberekening</t>
+  </si>
+  <si>
+    <t>verwijzing</t>
+  </si>
+  <si>
+    <r>
+      <t>Het in geld vastgesteld loon of het gedeelte dat overblijft na aftrek van hetgeen door de werkgever overeenkomstig </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>artikel 628 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mag worden verrekend, en na aftrek van hetgeen waarop derden overeenkomstig </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>artikel 633 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>rechten doen gelden, bedraagt €1235,-.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dit loon is niet voldaan uiterlijk de derde werkdag na die waarop ingevolge de artikelen 623 en 624 lid 1 de voldoening had moeten geschieden.</t>
+  </si>
+  <si>
+    <t>De aftrek van het loon, waarop derden overeenkomstig artikel 633 rechten doen gelden bedraagt  €0,-</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>Argument</t>
+  </si>
+  <si>
+    <t>[Argument]</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De werknemer heeft aanspraak op een verhoging. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +278,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -198,9 +308,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -505,20 +617,20 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,35 +646,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -575,7 +687,64 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,217 +754,423 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made Sequence.adl to demonstrate a total order.
This script works with Ampersand v3.1.0[master:fa51eef*]
</commit_message>
<xml_diff>
--- a/MirrorMe/Arguments.xlsx
+++ b/MirrorMe/Arguments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7305" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="7230" windowHeight="6855" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="2" r:id="rId1"/>
@@ -744,7 +744,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vereenvoudigde demo "Arguments.adl" met demo-script
</commit_message>
<xml_diff>
--- a/MirrorMe/Arguments.xlsx
+++ b/MirrorMe/Arguments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="7230" windowHeight="6855" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="2" r:id="rId1"/>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refinements in Execengine rules of MirrorMe
</commit_message>
<xml_diff>
--- a/MirrorMe/Arguments.xlsx
+++ b/MirrorMe/Arguments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="114">
   <si>
     <t>7148691</t>
   </si>
@@ -183,21 +183,9 @@
     <t>hetgeen door de werkgever overeenkomstig artikel 628 mag worden verrekend</t>
   </si>
   <si>
-    <t>Voor zover het in geld vastgesteld loon of het gedeelte dat overblijft na aftrek van hetgeen door de werkgever overeenkomstig artikel 628 mag worden verrekend, en na aftrek van hetgeen waarop derden overeenkomstig artikel 633 rechten doen gelden, niet wordt voldaan op uiterlijk de derde werkdag na de werkdag waarop ingevolge de artikelen 623 en 624 lid 1 de voldoening had moeten geschieden heeft de werknemer indien dit niet-voldoen aan de werkgever is toe te rekenen, aanspraak op een verhoging wegens vertraging.</t>
-  </si>
-  <si>
-    <t>De verhoging wegens vertraging bedraagt voor de vierde tot en met de achtste werkdag vijf procent per dag en voor elke volgende werkdag een procent, met dien verstande dat de verhoging wegens vertraging in geen geval de helft van [x1] te boven zal gaan.</t>
-  </si>
-  <si>
-    <t>Niettemin kan de rechter de verhoging wegens vertraging beperken tot zodanig bedrag als hem met het oog op de omstandigheden billijk zal voorkomen.</t>
-  </si>
-  <si>
     <t>verhoging wegens vertraging</t>
   </si>
   <si>
-    <t>Phrase</t>
-  </si>
-  <si>
     <t>Bavaria Transport, Hazerswoude</t>
   </si>
   <si>
@@ -324,21 +312,12 @@
     <t>descriptor</t>
   </si>
   <si>
-    <t>Tekst</t>
-  </si>
-  <si>
     <t>Regel</t>
   </si>
   <si>
     <t>warrant</t>
   </si>
   <si>
-    <t>tekst</t>
-  </si>
-  <si>
-    <t>refShowValue</t>
-  </si>
-  <si>
     <t>placeholder</t>
   </si>
   <si>
@@ -376,9 +355,6 @@
   </si>
   <si>
     <t>t1</t>
-  </si>
-  <si>
-    <t>verschuldigde, x2, werknemer, werkgever, verhoging</t>
   </si>
   <si>
     <t>[Identifier,]</t>
@@ -388,9 +364,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,12 +393,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -845,7 +816,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -858,10 +829,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F33" sqref="F33:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,853 +844,779 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>121</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" t="s">
-        <v>120</v>
-      </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" t="s">
-        <v>41</v>
+        <v>111</v>
+      </c>
+      <c r="F23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
+        <v>112</v>
+      </c>
+      <c r="D25" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E25" t="s">
         <v>18</v>
       </c>
-      <c r="G25" t="s">
-        <v>58</v>
+      <c r="F25" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D26" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E26" t="s">
         <v>18</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="D27" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
-      </c>
-      <c r="G27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
-      </c>
-      <c r="G28" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>33</v>
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
       </c>
-      <c r="G29" t="s">
-        <v>52</v>
+      <c r="F29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
-      </c>
-      <c r="G30" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="D31" s="3">
+        <v>42685.466099537036</v>
       </c>
       <c r="E31" t="s">
         <v>18</v>
       </c>
-      <c r="G31" t="s">
+      <c r="F31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35">
+        <v>400</v>
+      </c>
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>1235</v>
+      </c>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="2">
+        <v>42304</v>
+      </c>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40">
+        <v>617.5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="5">
-        <v>42685.466099537036</v>
-      </c>
-      <c r="E39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="5">
-        <v>42685.466099537036</v>
-      </c>
-      <c r="E40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="5">
-        <v>42685.466099537036</v>
-      </c>
-      <c r="E41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>1235</v>
+      </c>
+      <c r="H41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="5">
-        <v>42685.466099537036</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>1235</v>
+      </c>
+      <c r="H42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43" s="5">
-        <v>42685.466099537036</v>
+        <v>49</v>
       </c>
       <c r="E43" t="s">
         <v>18</v>
       </c>
-      <c r="F43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="5">
-        <v>42685.466099537036</v>
+        <v>51</v>
       </c>
       <c r="E44" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="2">
+        <v>42299</v>
+      </c>
+      <c r="H44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="5">
-        <v>42685.466099537036</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="F45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H48" t="s">
-        <v>75</v>
-      </c>
-      <c r="I48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-      <c r="H49">
-        <v>400</v>
-      </c>
-      <c r="I49" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" t="s">
-        <v>95</v>
-      </c>
-      <c r="F50">
-        <v>1235</v>
-      </c>
-      <c r="I50" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>39</v>
-      </c>
-      <c r="B51" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" s="2">
-        <v>42304</v>
-      </c>
-      <c r="I51" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" t="s">
-        <v>61</v>
-      </c>
-      <c r="I52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" t="s">
-        <v>84</v>
-      </c>
-      <c r="G53" t="s">
-        <v>72</v>
-      </c>
-      <c r="H53" t="s">
-        <v>60</v>
-      </c>
-      <c r="I53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" t="s">
-        <v>81</v>
-      </c>
-      <c r="H54">
-        <v>617.5</v>
-      </c>
-      <c r="I54" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" t="s">
-        <v>45</v>
-      </c>
-      <c r="G55" t="s">
-        <v>73</v>
-      </c>
-      <c r="H55">
-        <v>1235</v>
-      </c>
-      <c r="I55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>47</v>
-      </c>
-      <c r="B56" t="s">
-        <v>47</v>
-      </c>
-      <c r="F56">
-        <v>1235</v>
-      </c>
-      <c r="I56" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" t="s">
-        <v>49</v>
-      </c>
-      <c r="H57">
+      <c r="G45">
         <v>0</v>
       </c>
-      <c r="I57" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>51</v>
-      </c>
-      <c r="B58" t="s">
-        <v>51</v>
-      </c>
-      <c r="H58" s="2">
-        <v>42299</v>
-      </c>
-      <c r="I58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" t="s">
-        <v>53</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="H45" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>